<commit_message>
Wrapup and early geojson integration
</commit_message>
<xml_diff>
--- a/_reference/TNDM comparison.xlsx
+++ b/_reference/TNDM comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9120" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Lookup" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="165">
   <si>
     <t>Comparison of TNDM and QJM armour</t>
   </si>
@@ -520,6 +521,9 @@
   </si>
   <si>
     <t>M68</t>
+  </si>
+  <si>
+    <t>Bomb</t>
   </si>
 </sst>
 </file>
@@ -1056,11 +1060,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,39 +1128,39 @@
         <v>1</v>
       </c>
       <c r="B4" s="11">
-        <f>(B$37*B$33*B$35+B30)*B$28*B$25*B$26*B$27</f>
+        <f t="shared" ref="B4:J4" si="0">(B$37*B$33*B$35+B30)*B$28*B$25*B$26*B$27</f>
         <v>1737.8982628776864</v>
       </c>
       <c r="C4" s="11">
-        <f>(C$37*C$33*C$35+C30)*C$28*C$25*C$26*C$27</f>
+        <f t="shared" si="0"/>
         <v>952.72472602535493</v>
       </c>
       <c r="D4" s="11">
-        <f>(D$37*D$33*D$35+D30)*D$28*D$25*D$26*D$27</f>
+        <f t="shared" si="0"/>
         <v>518.29812443853655</v>
       </c>
       <c r="E4" s="11">
-        <f>(E$37*E$33*E$35+E30)*E$28*E$25*E$26*E$27</f>
+        <f t="shared" si="0"/>
         <v>1807.3188956409783</v>
       </c>
       <c r="F4" s="11">
-        <f>(F$37*F$33*F$35+F30)*F$28*F$25*F$26*F$27</f>
+        <f t="shared" si="0"/>
         <v>1823.2483192087036</v>
       </c>
       <c r="G4" s="11">
-        <f>(G$37*G$33*G$35+G30)*G$28*G$25*G$26*G$27</f>
+        <f t="shared" si="0"/>
         <v>12.036122416341822</v>
       </c>
       <c r="H4" s="11">
-        <f>(H$37*H$33*H$35+H30)*H$28*H$25*H$26*H$27</f>
+        <f t="shared" si="0"/>
         <v>305.15014353971145</v>
       </c>
       <c r="I4" s="11">
-        <f>(I$37*I$33*I$35+I30)*I$28*I$25*I$26*I$27</f>
+        <f t="shared" si="0"/>
         <v>525.58627181944212</v>
       </c>
       <c r="J4" s="11">
-        <f>(J$37*J$33*J$35+J30)*J$28*J$25*J$26*J$27</f>
+        <f t="shared" si="0"/>
         <v>149.15297394359763</v>
       </c>
     </row>
@@ -1165,39 +1169,39 @@
         <v>2</v>
       </c>
       <c r="B5" s="12">
-        <f>B38*B27*B36*B31*B34*B39</f>
+        <f t="shared" ref="B5:J5" si="1">B38*B27*B36*B31*B34*B39</f>
         <v>3157.569549712659</v>
       </c>
       <c r="C5" s="12">
-        <f>C38*C27*C36*C31*C34*C39</f>
+        <f t="shared" si="1"/>
         <v>966.05225510331672</v>
       </c>
       <c r="D5" s="12">
-        <f>D38*D27*D36*D31*D34*D39</f>
+        <f t="shared" si="1"/>
         <v>730.09551614664656</v>
       </c>
       <c r="E5" s="12">
-        <f>E38*E27*E36*E31*E34*E39</f>
+        <f t="shared" si="1"/>
         <v>3175.7551877149249</v>
       </c>
       <c r="F5" s="12">
-        <f>F38*F27*F36*F31*F34*F39</f>
+        <f t="shared" si="1"/>
         <v>3469.9216334605908</v>
       </c>
       <c r="G5" s="12">
-        <f>G38*G27*G36*G31*G34*G39</f>
+        <f t="shared" si="1"/>
         <v>8.323351717040623</v>
       </c>
       <c r="H5" s="12">
-        <f>H38*H27*H36*H31*H34*H39</f>
+        <f t="shared" si="1"/>
         <v>402.2143606265908</v>
       </c>
       <c r="I5" s="12">
-        <f>I38*I27*I36*I31*I34*I39</f>
+        <f t="shared" si="1"/>
         <v>670.86980332681799</v>
       </c>
       <c r="J5" s="12">
-        <f>J38*J27*J36*J31*J34*J39</f>
+        <f t="shared" si="1"/>
         <v>150.77027630829988</v>
       </c>
     </row>
@@ -1247,35 +1251,35 @@
         <v>106</v>
       </c>
       <c r="B7" s="11">
-        <f>(B$38*B$34*B$35*B31)*B$28*B$27*B39</f>
+        <f t="shared" ref="B7:J7" si="2">(B$38*B$34*B$35*B31)*B$28*B$27*B39</f>
         <v>3368.0741863601702</v>
       </c>
       <c r="C7" s="11">
-        <f t="shared" ref="C7" si="0">(C$38*C$34*C$35*C31)*C$28*C$27*C39</f>
+        <f t="shared" si="2"/>
         <v>1197.9047963281128</v>
       </c>
       <c r="D7" s="11">
-        <f t="shared" ref="D7:H7" si="1">(D$38*D$34*D$35*D31)*D$28*D$27*D39</f>
+        <f t="shared" si="2"/>
         <v>769.03394367446799</v>
       </c>
       <c r="E7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3387.4722002292538</v>
       </c>
       <c r="F7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3701.2497423579644</v>
       </c>
       <c r="G7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.9880220604487473</v>
       </c>
       <c r="H7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>429.02865133503025</v>
       </c>
       <c r="I7" s="11">
-        <f t="shared" ref="I7:J7" si="2">(I$38*I$34*I$35*I31)*I$28*I$27*I39</f>
+        <f t="shared" si="2"/>
         <v>805.04376399218143</v>
       </c>
       <c r="J7" s="11">
@@ -1957,39 +1961,39 @@
         <v>21</v>
       </c>
       <c r="B30" s="9">
-        <f>B20/4*SQRT(2*B20)</f>
+        <f t="shared" ref="B30:J30" si="3">B20/4*SQRT(2*B20)</f>
         <v>82.81907992727281</v>
       </c>
       <c r="C30" s="9">
-        <f>C20/4*SQRT(2*C20)</f>
+        <f t="shared" si="3"/>
         <v>144.21121662339584</v>
       </c>
       <c r="D30" s="9">
-        <f>D20/4*SQRT(2*D20)</f>
+        <f t="shared" si="3"/>
         <v>110.30412503619254</v>
       </c>
       <c r="E30" s="9">
-        <f>E20/4*SQRT(2*E20)</f>
+        <f t="shared" si="3"/>
         <v>140.29611541307906</v>
       </c>
       <c r="F30" s="9">
-        <f>F20/4*SQRT(2*F20)</f>
+        <f t="shared" si="3"/>
         <v>152.14836509144618</v>
       </c>
       <c r="G30" s="9">
-        <f>G20/4*SQRT(2*G20)</f>
+        <f t="shared" si="3"/>
         <v>6.5479004268543974</v>
       </c>
       <c r="H30" s="9">
-        <f>H20/4*SQRT(2*H20)</f>
+        <f t="shared" si="3"/>
         <v>76.367532368147124</v>
       </c>
       <c r="I30" s="9">
-        <f>I20/4*SQRT(2*I20)</f>
+        <f t="shared" si="3"/>
         <v>18.71904444676597</v>
       </c>
       <c r="J30" s="9">
-        <f>J20/4*SQRT(2*J20)</f>
+        <f t="shared" si="3"/>
         <v>18.71904444676597</v>
       </c>
     </row>
@@ -1998,39 +2002,39 @@
         <v>20</v>
       </c>
       <c r="B31" s="9">
-        <f>1.2*B23*B20/(2*B22*B21)</f>
+        <f t="shared" ref="B31:J31" si="4">1.2*B23*B20/(2*B22*B21)</f>
         <v>1.8939969925828306</v>
       </c>
       <c r="C31" s="9">
-        <f>1.2*C23*C20/(2*C22*C21)</f>
+        <f t="shared" si="4"/>
         <v>1.5132061628760087</v>
       </c>
       <c r="D31" s="9">
-        <f>1.2*D23*D20/(2*D22*D21)</f>
+        <f t="shared" si="4"/>
         <v>1.2417218543046358</v>
       </c>
       <c r="E31" s="9">
-        <f>1.2*E23*E20/(2*E22*E21)</f>
+        <f t="shared" si="4"/>
         <v>2.0931097926529261</v>
       </c>
       <c r="F31" s="9">
-        <f>1.2*F23*F20/(2*F22*F21)</f>
+        <f t="shared" si="4"/>
         <v>2.3021882041634796</v>
       </c>
       <c r="G31" s="9">
-        <f>1.2*G23*G20/(2*G22*G21)</f>
+        <f t="shared" si="4"/>
         <v>0.31620553359683795</v>
       </c>
       <c r="H31" s="9">
-        <f>1.2*H23*H20/(2*H22*H21)</f>
+        <f t="shared" si="4"/>
         <v>1.490066225165563</v>
       </c>
       <c r="I31" s="9">
-        <f>1.2*I23*I20/(2*I22*I21)</f>
+        <f t="shared" si="4"/>
         <v>0.51270396800145435</v>
       </c>
       <c r="J31" s="9">
-        <f>1.2*J23*J20/(2*J22*J21)</f>
+        <f t="shared" si="4"/>
         <v>0.51270396800145435</v>
       </c>
     </row>
@@ -2039,39 +2043,39 @@
         <v>18</v>
       </c>
       <c r="B32" s="9">
-        <f>B30*B24</f>
+        <f t="shared" ref="B32:J32" si="5">B30*B24</f>
         <v>107.66480390545466</v>
       </c>
       <c r="C32" s="9">
-        <f>C30*C24</f>
+        <f t="shared" si="5"/>
         <v>144.21121662339584</v>
       </c>
       <c r="D32" s="9">
-        <f>D30*D24</f>
+        <f t="shared" si="5"/>
         <v>110.30412503619254</v>
       </c>
       <c r="E32" s="9">
-        <f>E30*E24</f>
+        <f t="shared" si="5"/>
         <v>210.4441731196186</v>
       </c>
       <c r="F32" s="9">
-        <f>F30*F24</f>
+        <f t="shared" si="5"/>
         <v>228.22254763716927</v>
       </c>
       <c r="G32" s="9">
-        <f>G30*G24</f>
+        <f t="shared" si="5"/>
         <v>6.5479004268543974</v>
       </c>
       <c r="H32" s="9">
-        <f>H30*H24</f>
+        <f t="shared" si="5"/>
         <v>76.367532368147124</v>
       </c>
       <c r="I32" s="9">
-        <f>I30*I24</f>
+        <f t="shared" si="5"/>
         <v>18.71904444676597</v>
       </c>
       <c r="J32" s="9">
-        <f>J30*J24</f>
+        <f t="shared" si="5"/>
         <v>18.71904444676597</v>
       </c>
     </row>
@@ -2080,39 +2084,39 @@
         <v>16</v>
       </c>
       <c r="B33" s="13">
-        <f>0.15*SQRT(B16)</f>
+        <f t="shared" ref="B33:J33" si="6">0.15*SQRT(B16)</f>
         <v>1.1618950038622251</v>
       </c>
       <c r="C33" s="13">
-        <f>0.15*SQRT(C16)</f>
+        <f t="shared" si="6"/>
         <v>1.0392304845413263</v>
       </c>
       <c r="D33" s="13">
-        <f>0.15*SQRT(D16)</f>
+        <f t="shared" si="6"/>
         <v>1.0392304845413263</v>
       </c>
       <c r="E33" s="13">
-        <f>0.15*SQRT(E16)</f>
+        <f t="shared" si="6"/>
         <v>1.2549900398011133</v>
       </c>
       <c r="F33" s="13">
-        <f>0.15*SQRT(F16)</f>
+        <f t="shared" si="6"/>
         <v>1.2549900398011133</v>
       </c>
       <c r="G33" s="13">
-        <f>0.15*SQRT(G16)</f>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="H33" s="13">
-        <f>0.15*SQRT(H16)</f>
+        <f t="shared" si="6"/>
         <v>1.0392304845413263</v>
       </c>
       <c r="I33" s="13">
-        <f>0.15*SQRT(I16)</f>
+        <f t="shared" si="6"/>
         <v>1.2093386622447824</v>
       </c>
       <c r="J33" s="13">
-        <f>0.15*SQRT(J16)</f>
+        <f t="shared" si="6"/>
         <v>1.2093386622447824</v>
       </c>
     </row>
@@ -2121,39 +2125,39 @@
         <v>92</v>
       </c>
       <c r="B34" s="13">
-        <f>0.04*SQRT(B17/B20*B16/B18)</f>
+        <f t="shared" ref="B34:J34" si="7">0.04*SQRT(B17/B20*B16/B18)</f>
         <v>1.4544195362268579</v>
       </c>
       <c r="C34" s="13">
-        <f>0.04*SQRT(C17/C20*C16/C18)</f>
+        <f t="shared" si="7"/>
         <v>1.0787197799411874</v>
       </c>
       <c r="D34" s="13">
-        <f>0.04*SQRT(D17/D20*D16/D18)</f>
+        <f t="shared" si="7"/>
         <v>1.2503052875854532</v>
       </c>
       <c r="E34" s="13">
-        <f>0.04*SQRT(E17/E20*E16/E18)</f>
+        <f t="shared" si="7"/>
         <v>1.8106089164056556</v>
       </c>
       <c r="F34" s="13">
-        <f>0.04*SQRT(F17/F20*F16/F18)</f>
+        <f t="shared" si="7"/>
         <v>1.7623173091881328</v>
       </c>
       <c r="G34" s="13">
-        <f>0.04*SQRT(G17/G20*G16/G18)</f>
+        <f t="shared" si="7"/>
         <v>6.1721339984836767</v>
       </c>
       <c r="H34" s="13">
-        <f>0.04*SQRT(H17/H20*H16/H18)</f>
+        <f t="shared" si="7"/>
         <v>1.147550621098494</v>
       </c>
       <c r="I34" s="13">
-        <f>0.04*SQRT(I17/I20*I16/I18)</f>
+        <f t="shared" si="7"/>
         <v>1.8741203047249224</v>
       </c>
       <c r="J34" s="13">
-        <f>0.04*SQRT(J17/J20*J16/J18)</f>
+        <f t="shared" si="7"/>
         <v>1.8741203047249224</v>
       </c>
     </row>
@@ -2162,39 +2166,39 @@
         <v>24</v>
       </c>
       <c r="B35" s="13">
-        <f>0.08*SQRT(B19)</f>
+        <f t="shared" ref="B35:J35" si="8">0.08*SQRT(B19)</f>
         <v>1.7888543819998319</v>
       </c>
       <c r="C35" s="13">
-        <f>0.08*SQRT(C19)</f>
+        <f t="shared" si="8"/>
         <v>1.7888543819998319</v>
       </c>
       <c r="D35" s="13">
-        <f>0.08*SQRT(D19)</f>
+        <f t="shared" si="8"/>
         <v>1.7888543819998319</v>
       </c>
       <c r="E35" s="13">
-        <f>0.08*SQRT(E19)</f>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="F35" s="13">
-        <f>0.08*SQRT(F19)</f>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="G35" s="13">
-        <f>0.08*SQRT(G19)</f>
+        <f t="shared" si="8"/>
         <v>2.1908902300206647</v>
       </c>
       <c r="H35" s="13">
-        <f>0.08*SQRT(H19)</f>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="I35" s="13">
-        <f>0.08*SQRT(I19)</f>
+        <f t="shared" si="8"/>
         <v>1.9595917942265424</v>
       </c>
       <c r="J35" s="13">
-        <f>0.08*SQRT(J19)</f>
+        <f t="shared" si="8"/>
         <v>1.9595917942265424</v>
       </c>
     </row>
@@ -2203,39 +2207,39 @@
         <v>28</v>
       </c>
       <c r="B36" s="9">
-        <f>0.06*SQRT(B19)</f>
+        <f t="shared" ref="B36:J36" si="9">0.06*SQRT(B19)</f>
         <v>1.3416407864998738</v>
       </c>
       <c r="C36" s="9">
-        <f>0.06*SQRT(C19)</f>
+        <f t="shared" si="9"/>
         <v>1.3416407864998738</v>
       </c>
       <c r="D36" s="9">
-        <f>0.06*SQRT(D19)</f>
+        <f t="shared" si="9"/>
         <v>1.3416407864998738</v>
       </c>
       <c r="E36" s="9">
-        <f>0.06*SQRT(E19)</f>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="F36" s="9">
-        <f>0.06*SQRT(F19)</f>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="G36" s="9">
-        <f>0.06*SQRT(G19)</f>
+        <f t="shared" si="9"/>
         <v>1.6431676725154984</v>
       </c>
       <c r="H36" s="9">
-        <f>0.06*SQRT(H19)</f>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="I36" s="9">
-        <f>0.06*SQRT(I19)</f>
+        <f t="shared" si="9"/>
         <v>1.4696938456699067</v>
       </c>
       <c r="J36" s="9">
-        <f>0.06*SQRT(J19)</f>
+        <f t="shared" si="9"/>
         <v>1.4696938456699067</v>
       </c>
     </row>
@@ -2248,35 +2252,35 @@
         <v>997.04191000000003</v>
       </c>
       <c r="C37" s="8">
-        <f t="shared" ref="C37:H37" si="3">(C8+0.5*C9+0.33*C10+0.25*C11)/$H$1+C52</f>
+        <f t="shared" ref="C37:H37" si="10">(C8+0.5*C9+0.33*C10+0.25*C11)/$H$1+C52</f>
         <v>469.11162999999999</v>
       </c>
       <c r="D37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>407.47984000000002</v>
       </c>
       <c r="E37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>599.82308999999998</v>
       </c>
       <c r="F37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>599.82308999999998</v>
       </c>
       <c r="G37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>2.631875</v>
       </c>
       <c r="H37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>227.1662475</v>
       </c>
       <c r="I37" s="8">
-        <f t="shared" ref="I37:J37" si="4">(I8+0.5*I9+0.33*I10+0.25*I11)/$H$1+I52</f>
+        <f>(I8+0.5*I9+0.33*I10+0.25*I11)/$H$1+I52</f>
         <v>303.24599749999999</v>
       </c>
       <c r="J37" s="8">
-        <f t="shared" si="4"/>
+        <f>(J8+0.5*J9+0.33*J10+0.25*J11)/$H$1+J52</f>
         <v>80.398997500000007</v>
       </c>
     </row>
@@ -2289,35 +2293,35 @@
         <v>615.57204000000013</v>
       </c>
       <c r="C38" s="8">
-        <f t="shared" ref="C38:H38" si="5">SUMPRODUCT(C8:C11,C12:C15)/$H$1+C52</f>
+        <f t="shared" ref="C38:H38" si="11">SUMPRODUCT(C8:C11,C12:C15)/$H$1+C52</f>
         <v>376.15380000000005</v>
       </c>
       <c r="D38" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>327.41720000000009</v>
       </c>
       <c r="E38" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>481.71040000000011</v>
       </c>
       <c r="F38" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>481.71040000000011</v>
       </c>
       <c r="G38" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>2.4871249999999998</v>
       </c>
       <c r="H38" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>183.10379999999998</v>
       </c>
       <c r="I38" s="8">
-        <f t="shared" ref="I38:J38" si="6">SUMPRODUCT(I8:I11,I12:I15)/$H$1+I52</f>
+        <f>SUMPRODUCT(I8:I11,I12:I15)/$H$1+I52</f>
         <v>403.87405000000001</v>
       </c>
       <c r="J38" s="8">
-        <f t="shared" si="6"/>
+        <f>SUMPRODUCT(J8:J11,J12:J15)/$H$1+J52</f>
         <v>90.766050000000007</v>
       </c>
     </row>
@@ -2326,39 +2330,39 @@
         <v>32</v>
       </c>
       <c r="B39" s="13">
-        <f>SQRT(B40*B41*B42*B43*B44*B47*B48*B49*B50)</f>
+        <f t="shared" ref="B39:J39" si="12">SQRT(B40*B41*B42*B43*B44*B47*B48*B49*B50)</f>
         <v>1.3218418680954243</v>
       </c>
       <c r="C39" s="13">
-        <f>SQRT(C40*C41*C42*C43*C44*C47*C48*C49*C50)</f>
+        <f t="shared" si="12"/>
         <v>1.1168706281391771</v>
       </c>
       <c r="D39" s="13">
-        <f>SQRT(D40*D41*D42*D43*D44*D47*D48*D49*D50)</f>
+        <f t="shared" si="12"/>
         <v>1.0195587280779856</v>
       </c>
       <c r="E39" s="13">
-        <f>SQRT(E40*E41*E42*E43*E44*E47*E48*E49*E50)</f>
+        <f t="shared" si="12"/>
         <v>1.380618803652913</v>
       </c>
       <c r="F39" s="13">
-        <f>SQRT(F40*F41*F42*F43*F44*F47*F48*F49*F50)</f>
+        <f t="shared" si="12"/>
         <v>1.4090881659339136</v>
       </c>
       <c r="G39" s="13">
-        <f>SQRT(G40*G41*G42*G43*G44*G47*G48*G49*G50)</f>
+        <f t="shared" si="12"/>
         <v>0.94868329805051377</v>
       </c>
       <c r="H39" s="13">
-        <f>SQRT(H40*H41*H42*H43*H44*H47*H48*H49*H50)</f>
+        <f t="shared" si="12"/>
         <v>1.0195587280779856</v>
       </c>
       <c r="I39" s="13">
-        <f>SQRT(I40*I41*I42*I43*I44*I47*I48*I49*I50)</f>
+        <f t="shared" si="12"/>
         <v>1.069322215237297</v>
       </c>
       <c r="J39" s="13">
-        <f>SQRT(J40*J41*J42*J43*J44*J47*J48*J49*J50)</f>
+        <f t="shared" si="12"/>
         <v>1.069322215237297</v>
       </c>
     </row>
@@ -2547,39 +2551,39 @@
         <v>109</v>
       </c>
       <c r="B46" s="13">
-        <f>PRODUCT(B48:B50)*B41*B44*B43</f>
+        <f t="shared" ref="B46:J46" si="13">PRODUCT(B48:B50)*B41*B44*B43</f>
         <v>1.6808715000000007</v>
       </c>
       <c r="C46" s="13">
-        <f>PRODUCT(C48:C50)*C41*C44*C43</f>
+        <f t="shared" si="13"/>
         <v>1.26</v>
       </c>
       <c r="D46" s="13">
-        <f>PRODUCT(D48:D50)*D41*D44*D43</f>
+        <f t="shared" si="13"/>
         <v>1.05</v>
       </c>
       <c r="E46" s="13">
-        <f>PRODUCT(E48:E50)*E41*E44*E43</f>
+        <f t="shared" si="13"/>
         <v>1.8336780000000004</v>
       </c>
       <c r="F46" s="13">
-        <f>PRODUCT(F48:F50)*F41*F44*F43</f>
+        <f t="shared" si="13"/>
         <v>1.9100812500000004</v>
       </c>
       <c r="G46" s="13">
-        <f>PRODUCT(G48:G50)*G41*G44*G43</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="H46" s="13">
-        <f>PRODUCT(H48:H50)*H41*H44*H43</f>
+        <f t="shared" si="13"/>
         <v>1.05</v>
       </c>
       <c r="I46" s="13">
-        <f>PRODUCT(I48:I50)*I41*I44*I43</f>
+        <f t="shared" si="13"/>
         <v>1.1550000000000002</v>
       </c>
       <c r="J46" s="13">
-        <f>PRODUCT(J48:J50)*J41*J44*J43</f>
+        <f t="shared" si="13"/>
         <v>1.1550000000000002</v>
       </c>
     </row>
@@ -2733,39 +2737,39 @@
         <v>102</v>
       </c>
       <c r="B54" s="4">
-        <f>B57*B58*B60*B55*B61*B59</f>
+        <f t="shared" ref="B54:J54" si="14">B57*B58*B60*B55*B61*B59</f>
         <v>3157.569549712659</v>
       </c>
       <c r="C54" s="4">
-        <f>C57*C58*C60*C55*C61*C59</f>
+        <f t="shared" si="14"/>
         <v>966.05225510331661</v>
       </c>
       <c r="D54" s="4">
-        <f>D57*D58*D60*D55*D61*D59</f>
+        <f t="shared" si="14"/>
         <v>730.09551614664667</v>
       </c>
       <c r="E54" s="4">
-        <f>E57*E58*E60*E55*E61*E59</f>
+        <f t="shared" si="14"/>
         <v>3175.7551877149253</v>
       </c>
       <c r="F54" s="4">
-        <f>F57*F58*F60*F55*F61*F59</f>
+        <f t="shared" si="14"/>
         <v>3469.9216334605908</v>
       </c>
       <c r="G54" s="4">
-        <f>G57*G58*G60*G55*G61*G59</f>
+        <f t="shared" si="14"/>
         <v>8.323351717040623</v>
       </c>
       <c r="H54" s="4">
-        <f>H57*H58*H60*H55*H61*H59</f>
+        <f t="shared" si="14"/>
         <v>402.21436062659086</v>
       </c>
       <c r="I54">
-        <f>I57*I58*I60*I55*I61*I59</f>
+        <f t="shared" si="14"/>
         <v>670.86980332681799</v>
       </c>
       <c r="J54">
-        <f>J57*J58*J60*J55*J61*J59</f>
+        <f t="shared" si="14"/>
         <v>150.77027630829988</v>
       </c>
     </row>
@@ -2774,39 +2778,39 @@
         <v>104</v>
       </c>
       <c r="B55" s="4">
-        <f>B38</f>
+        <f t="shared" ref="B55:J55" si="15">B38</f>
         <v>615.57204000000013</v>
       </c>
       <c r="C55" s="4">
-        <f>C38</f>
+        <f t="shared" si="15"/>
         <v>376.15380000000005</v>
       </c>
       <c r="D55" s="4">
-        <f>D38</f>
+        <f t="shared" si="15"/>
         <v>327.41720000000009</v>
       </c>
       <c r="E55" s="4">
-        <f>E38</f>
+        <f t="shared" si="15"/>
         <v>481.71040000000011</v>
       </c>
       <c r="F55" s="4">
-        <f>F38</f>
+        <f t="shared" si="15"/>
         <v>481.71040000000011</v>
       </c>
       <c r="G55" s="4">
-        <f>G38</f>
+        <f t="shared" si="15"/>
         <v>2.4871249999999998</v>
       </c>
       <c r="H55" s="4">
-        <f>H38</f>
+        <f t="shared" si="15"/>
         <v>183.10379999999998</v>
       </c>
       <c r="I55">
-        <f>I38</f>
+        <f t="shared" si="15"/>
         <v>403.87405000000001</v>
       </c>
       <c r="J55">
-        <f>J38</f>
+        <f t="shared" si="15"/>
         <v>90.766050000000007</v>
       </c>
     </row>
@@ -2815,39 +2819,39 @@
         <v>111</v>
       </c>
       <c r="B56" s="3">
-        <f>PRODUCT(B57:B61)</f>
+        <f t="shared" ref="B56:J56" si="16">PRODUCT(B57:B61)</f>
         <v>5.1294882556924746</v>
       </c>
       <c r="C56" s="3">
-        <f>PRODUCT(C57:C61)</f>
+        <f t="shared" si="16"/>
         <v>2.5682373941279248</v>
       </c>
       <c r="D56" s="3">
-        <f>PRODUCT(D57:D61)</f>
+        <f t="shared" si="16"/>
         <v>2.2298630497928835</v>
       </c>
       <c r="E56" s="3">
-        <f>PRODUCT(E57:E61)</f>
+        <f t="shared" si="16"/>
         <v>6.5926647789105743</v>
       </c>
       <c r="F56" s="3">
-        <f>PRODUCT(F57:F61)</f>
+        <f t="shared" si="16"/>
         <v>7.2033355174822677</v>
       </c>
       <c r="G56" s="3">
-        <f>PRODUCT(G57:G61)</f>
+        <f t="shared" si="16"/>
         <v>3.3465755509034021</v>
       </c>
       <c r="H56" s="3">
-        <f>PRODUCT(H57:H61)</f>
+        <f t="shared" si="16"/>
         <v>2.1966467141948494</v>
       </c>
       <c r="I56">
-        <f>PRODUCT(I57:I61)</f>
+        <f t="shared" si="16"/>
         <v>1.6610866762219998</v>
       </c>
       <c r="J56">
-        <f>PRODUCT(J57:J61)</f>
+        <f t="shared" si="16"/>
         <v>1.6610866762219998</v>
       </c>
     </row>
@@ -2856,39 +2860,39 @@
         <v>26</v>
       </c>
       <c r="B57" s="4">
-        <f>B27</f>
+        <f t="shared" ref="B57:J57" si="17">B27</f>
         <v>1.05</v>
       </c>
       <c r="C57" s="4">
-        <f>C27</f>
+        <f t="shared" si="17"/>
         <v>1.05</v>
       </c>
       <c r="D57" s="4">
-        <f>D27</f>
+        <f t="shared" si="17"/>
         <v>1.05</v>
       </c>
       <c r="E57" s="4">
-        <f>E27</f>
+        <f t="shared" si="17"/>
         <v>1.05</v>
       </c>
       <c r="F57" s="4">
-        <f>F27</f>
+        <f t="shared" si="17"/>
         <v>1.05</v>
       </c>
       <c r="G57" s="4">
-        <f>G27</f>
+        <f t="shared" si="17"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="H57" s="4">
-        <f>H27</f>
+        <f t="shared" si="17"/>
         <v>1.05</v>
       </c>
       <c r="I57">
-        <f>I27</f>
+        <f t="shared" si="17"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="J57">
-        <f>J27</f>
+        <f t="shared" si="17"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -2897,39 +2901,39 @@
         <v>10</v>
       </c>
       <c r="B58" s="4">
-        <f>B31</f>
+        <f t="shared" ref="B58:J58" si="18">B31</f>
         <v>1.8939969925828306</v>
       </c>
       <c r="C58" s="4">
-        <f>C31</f>
+        <f t="shared" si="18"/>
         <v>1.5132061628760087</v>
       </c>
       <c r="D58" s="4">
-        <f>D31</f>
+        <f t="shared" si="18"/>
         <v>1.2417218543046358</v>
       </c>
       <c r="E58" s="4">
-        <f>E31</f>
+        <f t="shared" si="18"/>
         <v>2.0931097926529261</v>
       </c>
       <c r="F58" s="4">
-        <f>F31</f>
+        <f t="shared" si="18"/>
         <v>2.3021882041634796</v>
       </c>
       <c r="G58" s="4">
-        <f>G31</f>
+        <f t="shared" si="18"/>
         <v>0.31620553359683795</v>
       </c>
       <c r="H58" s="4">
-        <f>H31</f>
+        <f t="shared" si="18"/>
         <v>1.490066225165563</v>
       </c>
       <c r="I58">
-        <f>I31</f>
+        <f t="shared" si="18"/>
         <v>0.51270396800145435</v>
       </c>
       <c r="J58">
-        <f>J31</f>
+        <f t="shared" si="18"/>
         <v>0.51270396800145435</v>
       </c>
     </row>
@@ -2938,39 +2942,39 @@
         <v>103</v>
       </c>
       <c r="B59" s="4">
-        <f>B34</f>
+        <f t="shared" ref="B59:J59" si="19">B34</f>
         <v>1.4544195362268579</v>
       </c>
       <c r="C59" s="4">
-        <f>C34</f>
+        <f t="shared" si="19"/>
         <v>1.0787197799411874</v>
       </c>
       <c r="D59" s="4">
-        <f>D34</f>
+        <f t="shared" si="19"/>
         <v>1.2503052875854532</v>
       </c>
       <c r="E59" s="4">
-        <f>E34</f>
+        <f t="shared" si="19"/>
         <v>1.8106089164056556</v>
       </c>
       <c r="F59" s="4">
-        <f>F34</f>
+        <f t="shared" si="19"/>
         <v>1.7623173091881328</v>
       </c>
       <c r="G59" s="4">
-        <f>G34</f>
+        <f t="shared" si="19"/>
         <v>6.1721339984836767</v>
       </c>
       <c r="H59" s="4">
-        <f>H34</f>
+        <f t="shared" si="19"/>
         <v>1.147550621098494</v>
       </c>
       <c r="I59">
-        <f>I34</f>
+        <f t="shared" si="19"/>
         <v>1.8741203047249224</v>
       </c>
       <c r="J59">
-        <f>J34</f>
+        <f t="shared" si="19"/>
         <v>1.8741203047249224</v>
       </c>
     </row>
@@ -2979,39 +2983,39 @@
         <v>105</v>
       </c>
       <c r="B60" s="4">
-        <f>B36</f>
+        <f t="shared" ref="B60:J60" si="20">B36</f>
         <v>1.3416407864998738</v>
       </c>
       <c r="C60" s="4">
-        <f>C36</f>
+        <f t="shared" si="20"/>
         <v>1.3416407864998738</v>
       </c>
       <c r="D60" s="4">
-        <f>D36</f>
+        <f t="shared" si="20"/>
         <v>1.3416407864998738</v>
       </c>
       <c r="E60" s="4">
-        <f>E36</f>
+        <f t="shared" si="20"/>
         <v>1.2</v>
       </c>
       <c r="F60" s="4">
-        <f>F36</f>
+        <f t="shared" si="20"/>
         <v>1.2</v>
       </c>
       <c r="G60" s="4">
-        <f>G36</f>
+        <f t="shared" si="20"/>
         <v>1.6431676725154984</v>
       </c>
       <c r="H60" s="4">
-        <f>H36</f>
+        <f t="shared" si="20"/>
         <v>1.2</v>
       </c>
       <c r="I60">
-        <f>I36</f>
+        <f t="shared" si="20"/>
         <v>1.4696938456699067</v>
       </c>
       <c r="J60">
-        <f>J36</f>
+        <f t="shared" si="20"/>
         <v>1.4696938456699067</v>
       </c>
     </row>
@@ -3020,39 +3024,39 @@
         <v>31</v>
       </c>
       <c r="B61" s="4">
-        <f>B39</f>
+        <f t="shared" ref="B61:J61" si="21">B39</f>
         <v>1.3218418680954243</v>
       </c>
       <c r="C61" s="4">
-        <f>C39</f>
+        <f t="shared" si="21"/>
         <v>1.1168706281391771</v>
       </c>
       <c r="D61" s="4">
-        <f>D39</f>
+        <f t="shared" si="21"/>
         <v>1.0195587280779856</v>
       </c>
       <c r="E61" s="4">
-        <f>E39</f>
+        <f t="shared" si="21"/>
         <v>1.380618803652913</v>
       </c>
       <c r="F61" s="4">
-        <f>F39</f>
+        <f t="shared" si="21"/>
         <v>1.4090881659339136</v>
       </c>
       <c r="G61" s="4">
-        <f>G39</f>
+        <f t="shared" si="21"/>
         <v>0.94868329805051377</v>
       </c>
       <c r="H61" s="4">
-        <f>H39</f>
+        <f t="shared" si="21"/>
         <v>1.0195587280779856</v>
       </c>
       <c r="I61">
-        <f>I39</f>
+        <f t="shared" si="21"/>
         <v>1.069322215237297</v>
       </c>
       <c r="J61">
-        <f>J39</f>
+        <f t="shared" si="21"/>
         <v>1.069322215237297</v>
       </c>
     </row>
@@ -3066,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3102,38 +3106,40 @@
       <c r="G2" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="21" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>126</v>
       </c>
       <c r="B3" s="11">
-        <f ca="1">PRODUCT(B5:B16)</f>
+        <f t="shared" ref="B3:H3" ca="1" si="0">PRODUCT(B5:B16)</f>
         <v>896994</v>
       </c>
       <c r="C3" s="11">
-        <f ca="1">PRODUCT(C5:C16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2747.7223787877074</v>
       </c>
       <c r="D3" s="11">
-        <f ca="1">PRODUCT(D5:D16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6374.3865533306971</v>
       </c>
       <c r="E3" s="11">
-        <f ca="1">PRODUCT(E5:E16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>281159.13410878187</v>
       </c>
       <c r="F3" s="11">
-        <f ca="1">PRODUCT(F5:F16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2393302.1357578584</v>
       </c>
       <c r="G3" s="11">
-        <f ca="1">PRODUCT(G5:G16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1463400.8326642646</v>
       </c>
       <c r="H3" s="11" t="e">
-        <f ca="1">PRODUCT(H5:H16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -3146,27 +3152,27 @@
         <v>1034500.5763767173</v>
       </c>
       <c r="C4" s="11">
-        <f t="shared" ref="C4:H4" ca="1" si="0">PRODUCT(C5:C16)*C34</f>
+        <f t="shared" ref="C4:H4" ca="1" si="1">PRODUCT(C5:C16)*C34</f>
         <v>2747.7223787877074</v>
       </c>
       <c r="D4" s="11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6374.3865533306971</v>
       </c>
       <c r="E4" s="11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>293732.9528360262</v>
       </c>
       <c r="F4" s="11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2814686.4597469182</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1741061.6183246253</v>
       </c>
       <c r="H4" s="11" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -3175,31 +3181,31 @@
         <v>125</v>
       </c>
       <c r="B5" s="8">
-        <f ca="1">IF(B20=0,B17,B20*B21)</f>
+        <f t="shared" ref="B5:H5" ca="1" si="2">IF(B20=0,B17,B20*B21)</f>
         <v>120</v>
       </c>
       <c r="C5" s="8">
-        <f>IF(C20=0,C17,C20*C21)</f>
+        <f t="shared" si="2"/>
         <v>3200</v>
       </c>
       <c r="D5" s="8">
-        <f>IF(D20=0,D17,D20*D21)</f>
+        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
       <c r="E5" s="8">
-        <f>IF(E20=0,E17,E20*E21)</f>
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="F5" s="8">
-        <f ca="1">IF(F20=0,F17,F20*F21)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>94.5</v>
       </c>
       <c r="G5" s="8">
-        <f ca="1">IF(G20=0,G17,G20*G21)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>113</v>
       </c>
       <c r="H5" s="8" t="e">
-        <f ca="1">IF(H20=0,H17,H20*H21)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -3241,31 +3247,31 @@
         <v>127</v>
       </c>
       <c r="B7" s="24">
-        <f>B23</f>
+        <f t="shared" ref="B7:H7" si="3">B23</f>
         <v>1</v>
       </c>
       <c r="C7" s="24">
-        <f>C23</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
       <c r="D7" s="24">
-        <f>D23</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E7" s="24">
-        <f>E23</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F7" s="24">
-        <f>F23</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G7" s="24">
-        <f>G23</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H7" s="24">
-        <f>H23</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3278,27 +3284,27 @@
         <v>7.0000000000000009</v>
       </c>
       <c r="C8" s="24">
-        <f t="shared" ref="C8:H8" si="1">IF(C19&gt;C18,C19,(C18+C19)/2)</f>
+        <f t="shared" ref="C8:H8" si="4">IF(C19&gt;C18,C19,(C18+C19)/2)</f>
         <v>1.7036969114507114</v>
       </c>
       <c r="D8" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.1079320612866064</v>
       </c>
       <c r="E8" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.7190361654600781</v>
       </c>
       <c r="F8" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>14.087228258248675</v>
       </c>
       <c r="G8" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.76647116979375</v>
       </c>
       <c r="H8" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3307,31 +3313,31 @@
         <v>129</v>
       </c>
       <c r="B9" s="13">
-        <f>B25</f>
+        <f t="shared" ref="B9:H10" si="5">B25</f>
         <v>0.9</v>
       </c>
       <c r="C9" s="13">
-        <f>C25</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="D9" s="13">
-        <f>D25</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="E9" s="13">
-        <f>E25</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="F9" s="13">
-        <f>F25</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="G9" s="13">
-        <f>G25</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="H9" s="13">
-        <f>H25</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3340,31 +3346,31 @@
         <v>130</v>
       </c>
       <c r="B10" s="13">
-        <f>B26</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="C10" s="13">
-        <f>C26</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="D10" s="13">
-        <f>D26</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="E10" s="13">
-        <f>E26</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="F10" s="13">
-        <f>F26</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="G10" s="13">
-        <f>G26</f>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="H10" s="13">
-        <f>H26</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3562,31 +3568,31 @@
         <v>128</v>
       </c>
       <c r="B18" s="26">
-        <f>1+SQRT(0.001*B24)</f>
+        <f t="shared" ref="B18:H18" si="6">1+SQRT(0.001*B24)</f>
         <v>2.7320508075688772</v>
       </c>
       <c r="C18" s="26">
-        <f>1+SQRT(0.001*C24)</f>
+        <f t="shared" si="6"/>
         <v>1.7745966692414834</v>
       </c>
       <c r="D18" s="26">
-        <f>1+SQRT(0.001*D24)</f>
+        <f t="shared" si="6"/>
         <v>1.8944271909999157</v>
       </c>
       <c r="E18" s="26">
-        <f>1+SQRT(0.001*E24)</f>
+        <f t="shared" si="6"/>
         <v>2.58113883008419</v>
       </c>
       <c r="F18" s="26">
-        <f>1+SQRT(0.001*F24)</f>
+        <f t="shared" si="6"/>
         <v>2.7320508075688772</v>
       </c>
       <c r="G18" s="26">
-        <f>1+SQRT(0.001*G24)</f>
+        <f t="shared" si="6"/>
         <v>2.7320508075688772</v>
       </c>
       <c r="H18" s="26">
-        <f>1+SQRT(0.001*H24)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3599,27 +3605,27 @@
         <v>7.0000000000000009</v>
       </c>
       <c r="C19" s="13">
-        <f t="shared" ref="C19:H19" si="2">0.007*C27*0.1*SQRT(C22)</f>
+        <f t="shared" ref="C19:H19" si="7">0.007*C27*0.1*SQRT(C22)</f>
         <v>1.6327971536599395</v>
       </c>
       <c r="D19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.1079320612866064</v>
       </c>
       <c r="E19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3.7190361654600781</v>
       </c>
       <c r="F19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>14.087228258248675</v>
       </c>
       <c r="G19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>10.76647116979375</v>
       </c>
       <c r="H19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3809,7 +3815,9 @@
       <c r="G27" s="32">
         <v>1501</v>
       </c>
-      <c r="H27" s="32"/>
+      <c r="H27" s="32">
+        <v>300</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
@@ -3852,31 +3860,31 @@
         <v>120</v>
       </c>
       <c r="B30" s="13">
-        <f ca="1">B29/B5</f>
+        <f t="shared" ref="B30:H30" ca="1" si="8">B29/B5</f>
         <v>0.35833333333333334</v>
       </c>
       <c r="C30" s="13">
-        <f>C29/C5</f>
+        <f t="shared" si="8"/>
         <v>0.625</v>
       </c>
       <c r="D30" s="13">
-        <f>D29/D5</f>
+        <f t="shared" si="8"/>
         <v>0.25</v>
       </c>
       <c r="E30" s="13">
-        <f>E29/E5</f>
+        <f t="shared" si="8"/>
         <v>0.25</v>
       </c>
       <c r="F30" s="13">
-        <f ca="1">F29/F5</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="G30" s="13">
-        <f ca="1">G29/G5</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.48672566371681414</v>
       </c>
       <c r="H30" s="13" t="e">
-        <f ca="1">H29/H5</f>
+        <f t="shared" ca="1" si="8"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -3955,27 +3963,27 @@
         <v>1.1532970971675589</v>
       </c>
       <c r="C34" s="13">
-        <f t="shared" ref="C34:H34" si="3">1+0.01*SQRT(ABS(C35))</f>
+        <f t="shared" ref="C34:H34" si="9">1+0.01*SQRT(ABS(C35))</f>
         <v>1</v>
       </c>
       <c r="D34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.0447213595499958</v>
       </c>
       <c r="F34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1760681686165901</v>
       </c>
       <c r="G34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1897366596101029</v>
       </c>
       <c r="H34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>